<commit_message>
refining the carbon storage chart (based on test area file)
</commit_message>
<xml_diff>
--- a/carbon_stock_cfs/carbon_storage_ton_C_per_hectare.xlsx
+++ b/carbon_stock_cfs/carbon_storage_ton_C_per_hectare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\catli\Documents\ESM 244 Labs\esm244-final-project\carbon_stock_cfs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D418B31-DEDC-428D-B5D3-C3408B635613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C34863-5273-4D84-AF6B-C152F6A6DD87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="384" windowWidth="21468" windowHeight="9552" xr2:uid="{FED94ABA-A127-4349-9A47-2E5BE6707665}"/>
   </bookViews>
@@ -540,7 +540,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>